<commit_message>
Update preprint link and figures for submission
</commit_message>
<xml_diff>
--- a/manuscript/supplemental_materials/supplemental_tables.xlsx
+++ b/manuscript/supplemental_materials/supplemental_tables.xlsx
@@ -701,25 +701,25 @@
         <v>3244</v>
       </c>
       <c r="F2">
-        <v>0.00546494749256711</v>
+        <v>0.06323030329795815</v>
       </c>
       <c r="G2">
-        <v>0.01175158957474063</v>
+        <v>0.07037971275265195</v>
       </c>
       <c r="H2">
-        <v>1.016537817973561</v>
+        <v>1.156045626882784</v>
       </c>
       <c r="I2">
         <v>10</v>
       </c>
       <c r="J2">
-        <v>0.748957982554907</v>
+        <v>0.9087589758219556</v>
       </c>
       <c r="K2">
-        <v>1.02892606304589</v>
+        <v>1.227149368580355</v>
       </c>
       <c r="L2">
-        <v>1.039608363493345</v>
+        <v>1.182282332282601</v>
       </c>
     </row>
     <row r="3">
@@ -739,31 +739,31 @@
         </is>
       </c>
       <c r="D3">
-        <v>0.0369801736728461</v>
+        <v>0.03698017367284619</v>
       </c>
       <c r="E3">
         <v>503</v>
       </c>
       <c r="F3">
-        <v>-0.05013492940643528</v>
+        <v>1.624880647527778E-17</v>
       </c>
       <c r="G3">
-        <v>-0.00762990432429362</v>
+        <v>0.0483383377361283</v>
       </c>
       <c r="H3">
-        <v>0.8793232674687781</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>10</v>
       </c>
       <c r="J3">
-        <v>0.748957982554907</v>
+        <v>0.9087589758219556</v>
       </c>
       <c r="K3">
-        <v>1.02892606304589</v>
+        <v>1.227149368580355</v>
       </c>
       <c r="L3">
-        <v>1.039608363493345</v>
+        <v>1.182282332282601</v>
       </c>
     </row>
     <row r="4">
@@ -783,31 +783,31 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.2457027970847805</v>
+        <v>0.2457027970847806</v>
       </c>
       <c r="E4">
         <v>503</v>
       </c>
       <c r="F4">
-        <v>-0.05013492940643528</v>
+        <v>1.624880647527778E-17</v>
       </c>
       <c r="G4">
-        <v>-0.00762990432429362</v>
+        <v>0.0483383377361283</v>
       </c>
       <c r="H4">
-        <v>0.8793232674687781</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>3244</v>
       </c>
       <c r="J4">
-        <v>0.00546494749256711</v>
+        <v>0.06323030329795815</v>
       </c>
       <c r="K4">
-        <v>0.01175158957474063</v>
+        <v>0.07037971275265195</v>
       </c>
       <c r="L4">
-        <v>1.016537817973561</v>
+        <v>1.156045626882784</v>
       </c>
     </row>
     <row r="5">
@@ -833,25 +833,25 @@
         <v>3244</v>
       </c>
       <c r="F5">
-        <v>-0.0964599779891071</v>
+        <v>-0.8454869057313058</v>
       </c>
       <c r="G5">
-        <v>-0.09369933640081184</v>
+        <v>-0.8424127351576889</v>
       </c>
       <c r="H5">
-        <v>0.9709224710163</v>
+        <v>1.081191163067631</v>
       </c>
       <c r="I5">
         <v>10</v>
       </c>
       <c r="J5">
-        <v>-2.047086226253547</v>
+        <v>-3.017647840335809</v>
       </c>
       <c r="K5">
-        <v>-2.044003401359202</v>
+        <v>-3.014214895757277</v>
       </c>
       <c r="L5">
-        <v>0.3286127296044282</v>
+        <v>0.3659336249041001</v>
       </c>
     </row>
     <row r="6">
@@ -871,31 +871,31 @@
         </is>
       </c>
       <c r="D6">
-        <v>3.02126384923739E-18</v>
+        <v>3.021263849237435E-18</v>
       </c>
       <c r="E6">
         <v>503</v>
       </c>
       <c r="F6">
-        <v>0.6627972780500968</v>
+        <v>3.148475688524556E-16</v>
       </c>
       <c r="G6">
-        <v>0.6262948691605261</v>
+        <v>-0.04064802607851307</v>
       </c>
       <c r="H6">
-        <v>0.8980118448818346</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>10</v>
       </c>
       <c r="J6">
-        <v>-2.047086226253547</v>
+        <v>-3.017647840335809</v>
       </c>
       <c r="K6">
-        <v>-2.044003401359202</v>
+        <v>-3.014214895757277</v>
       </c>
       <c r="L6">
-        <v>0.3286127296044282</v>
+        <v>0.3659336249041001</v>
       </c>
     </row>
     <row r="7">
@@ -921,25 +921,25 @@
         <v>503</v>
       </c>
       <c r="F7">
-        <v>0.6627972780500968</v>
+        <v>3.148475688524556E-16</v>
       </c>
       <c r="G7">
-        <v>0.6262948691605261</v>
+        <v>-0.04064802607851307</v>
       </c>
       <c r="H7">
-        <v>0.8980118448818346</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>3244</v>
       </c>
       <c r="J7">
-        <v>-0.0964599779891071</v>
+        <v>-0.8454869057313058</v>
       </c>
       <c r="K7">
-        <v>-0.09369933640081184</v>
+        <v>-0.8424127351576889</v>
       </c>
       <c r="L7">
-        <v>0.9709224710163</v>
+        <v>1.081191163067631</v>
       </c>
     </row>
     <row r="8">
@@ -965,25 +965,25 @@
         <v>3244</v>
       </c>
       <c r="F8">
-        <v>0.0112112621925764</v>
+        <v>0.0956191308383743</v>
       </c>
       <c r="G8">
-        <v>0.0292898185554143</v>
+        <v>0.1172182842945411</v>
       </c>
       <c r="H8">
-        <v>1.023016012647069</v>
+        <v>1.222236964158308</v>
       </c>
       <c r="I8">
         <v>10</v>
       </c>
       <c r="J8">
-        <v>-0.175174897999425</v>
+        <v>-0.1270636539645138</v>
       </c>
       <c r="K8">
-        <v>-0.08840190136216469</v>
+        <v>-0.02339258462668434</v>
       </c>
       <c r="L8">
-        <v>0.8953567439167825</v>
+        <v>1.069717477531852</v>
       </c>
     </row>
     <row r="9">
@@ -1009,25 +1009,25 @@
         <v>503</v>
       </c>
       <c r="F9">
-        <v>-0.06882223771913304</v>
+        <v>7.939075796703894E-17</v>
       </c>
       <c r="G9">
-        <v>-0.02830432748905981</v>
+        <v>0.04840832106381549</v>
       </c>
       <c r="H9">
-        <v>0.8370030056745725</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <v>10</v>
       </c>
       <c r="J9">
-        <v>-0.175174897999425</v>
+        <v>-0.1270636539645138</v>
       </c>
       <c r="K9">
-        <v>-0.08840190136216469</v>
+        <v>-0.02339258462668434</v>
       </c>
       <c r="L9">
-        <v>0.8953567439167825</v>
+        <v>1.069717477531852</v>
       </c>
     </row>
     <row r="10">
@@ -1047,31 +1047,31 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.284776849455003</v>
+        <v>0.2847768494550035</v>
       </c>
       <c r="E10">
         <v>503</v>
       </c>
       <c r="F10">
-        <v>-0.06882223771913304</v>
+        <v>7.939075796703894E-17</v>
       </c>
       <c r="G10">
-        <v>-0.02830432748905981</v>
+        <v>0.04840832106381549</v>
       </c>
       <c r="H10">
-        <v>0.8370030056745725</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <v>3244</v>
       </c>
       <c r="J10">
-        <v>0.0112112621925764</v>
+        <v>0.0956191308383743</v>
       </c>
       <c r="K10">
-        <v>0.0292898185554143</v>
+        <v>0.1172182842945411</v>
       </c>
       <c r="L10">
-        <v>1.023016012647069</v>
+        <v>1.222236964158308</v>
       </c>
     </row>
   </sheetData>
@@ -6599,7 +6599,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6688,54 +6688,87 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>log10(brain_mass_g)</t>
+          <t>vocal_learner_binary</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>HAQER_sequence_similarity_scaled</t>
+          <t>HAR_sequence_similarity_scaled</t>
         </is>
       </c>
       <c r="C3">
-        <v>0.4249453628485422</v>
+        <v>-0.1540054806338727</v>
       </c>
       <c r="D3">
-        <v>0.1522033550779373</v>
+        <v>0.3558521948819901</v>
       </c>
       <c r="E3">
-        <v>2.791957921235997</v>
+        <v>-0.4327793472931786</v>
       </c>
       <c r="F3">
-        <v>0.00614504692212833</v>
+        <v>0.6651750786189072</v>
       </c>
       <c r="G3">
-        <v>116</v>
+        <v>170</v>
+      </c>
+      <c r="H3">
+        <v>49</v>
+      </c>
+      <c r="I3">
+        <v>121</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>log10(brain_mass_g)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>HAQER_sequence_similarity_scaled</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>0.4249453628485422</v>
+      </c>
+      <c r="D4">
+        <v>0.1522033550779373</v>
+      </c>
+      <c r="E4">
+        <v>2.791957921235997</v>
+      </c>
+      <c r="F4">
+        <v>0.00614504692212833</v>
+      </c>
+      <c r="G4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>birth_weight_to_adult_weight_ratio</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>HAQER_sequence_similarity_scaled</t>
         </is>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>0.4420266527009095</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>0.1327971703179547</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>3.32858487603742</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>0.00117891670261702</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>115</v>
       </c>
     </row>

</xml_diff>